<commit_message>
Added Robin's part #'s. Needs MAXIM POE Controller supplier.
</commit_message>
<xml_diff>
--- a/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
+++ b/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$67</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="294">
   <si>
     <t>Qty</t>
   </si>
@@ -831,9 +831,6 @@
     <t>PCE3497CT-ND </t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>1N4448W-FDICT-ND</t>
   </si>
   <si>
@@ -856,9 +853,6 @@
   </si>
   <si>
     <t>LMZ14202HTZ/NOPBCT-ND</t>
-  </si>
-  <si>
-    <t>Not poulated</t>
   </si>
   <si>
     <t>SMAJ58ALFTR-ND</t>
@@ -896,13 +890,25 @@
   <si>
     <t>NON-DIGIKEY
 ITEMS</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>670-1190-1-ND</t>
+  </si>
+  <si>
+    <t>Not populated</t>
+  </si>
+  <si>
+    <t>CKN9104CT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,13 +945,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -960,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -976,6 +995,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1273,7 +1301,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="146.85546875" defaultRowHeight="15"/>
   <cols>
@@ -1346,33 +1376,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="B2" s="3">
+    <row r="2" spans="1:16" s="6" customFormat="1">
+      <c r="B2" s="6">
         <f>H2*3</f>
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1400,27 +1430,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="B4" s="3">
+    <row r="4" spans="1:16" s="6" customFormat="1">
+      <c r="B4" s="6">
         <f>H4*3</f>
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1470,7 +1500,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="3">
-        <f>H7*3</f>
+        <f t="shared" ref="B7:B38" si="0">H7*3</f>
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1497,7 +1527,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="B8" s="3">
-        <f>H8*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1524,7 +1554,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="3">
-        <f>H9*3</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1551,7 +1581,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="B10" s="3">
-        <f>H10*3</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1578,7 +1608,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="B11" s="3">
-        <f>H11*3</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1605,7 +1635,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="3">
-        <f>H12*3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1632,7 +1662,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="B13" s="3">
-        <f>H13*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1659,7 +1689,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="B14" s="3">
-        <f>H14*3</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1686,14 +1716,14 @@
     </row>
     <row r="15" spans="1:16">
       <c r="B15" s="3">
-        <f>H15*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>52</v>
@@ -1713,7 +1743,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="3">
-        <f>H16*3</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1740,7 +1770,7 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="3">
-        <f>H17*3</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1767,7 +1797,7 @@
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="3">
-        <f>H18*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1794,7 +1824,7 @@
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="3">
-        <f>H19*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1821,7 +1851,7 @@
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="3">
-        <f>H20*3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1848,14 +1878,14 @@
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="3">
-        <f>H21*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>67</v>
@@ -1878,14 +1908,14 @@
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="3">
-        <f>H22*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>74</v>
@@ -1908,7 +1938,7 @@
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="3">
-        <f>H23*3</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1935,7 +1965,7 @@
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="3">
-        <f>H24*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1965,7 +1995,7 @@
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="3">
-        <f>H25*3</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1992,7 +2022,7 @@
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="3">
-        <f>H26*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2019,7 +2049,7 @@
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="3">
-        <f>H27*3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2046,7 +2076,7 @@
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="3">
-        <f>H28*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2073,11 +2103,11 @@
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="3">
-        <f>H29*3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>96</v>
@@ -2097,7 +2127,7 @@
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="3">
-        <f>H30*3</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2124,7 +2154,7 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="3">
-        <f>H31*3</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -2151,7 +2181,7 @@
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="3">
-        <f>H32*3</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2178,7 +2208,7 @@
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="3">
-        <f>H33*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2205,7 +2235,7 @@
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="3">
-        <f>H34*3</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -2232,7 +2262,7 @@
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="3">
-        <f>H35*3</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2259,7 +2289,7 @@
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="3">
-        <f>H36*3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2286,7 +2316,7 @@
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="3">
-        <f>H37*3</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2313,7 +2343,7 @@
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="3">
-        <f>H38*3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2340,7 +2370,7 @@
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="3">
-        <f>H39*3</f>
+        <f t="shared" ref="B39:B67" si="1">H39*3</f>
         <v>30</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2367,7 +2397,7 @@
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="3">
-        <f>H40*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2394,7 +2424,7 @@
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="3">
-        <f>H41*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2421,7 +2451,7 @@
     </row>
     <row r="42" spans="2:10">
       <c r="B42" s="3">
-        <f>H42*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -2448,7 +2478,7 @@
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="3">
-        <f>H43*3</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2475,7 +2505,7 @@
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="3">
-        <f>H44*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2502,7 +2532,7 @@
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="3">
-        <f>H45*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2529,7 +2559,7 @@
     </row>
     <row r="46" spans="2:10">
       <c r="B46" s="3">
-        <f>H46*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -2556,7 +2586,7 @@
     </row>
     <row r="47" spans="2:10">
       <c r="B47" s="3">
-        <f>H47*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2583,7 +2613,7 @@
     </row>
     <row r="48" spans="2:10">
       <c r="B48" s="3">
-        <f>H48*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -2608,9 +2638,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:14">
       <c r="B49" s="3">
-        <f>H49*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2635,9 +2665,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:14">
       <c r="B50" s="3">
-        <f>H50*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2662,9 +2692,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="2:16">
+    <row r="51" spans="2:14">
       <c r="B51" s="3">
-        <f>H51*3</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2689,9 +2719,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:14">
       <c r="B52" s="3">
-        <f>H52*3</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2716,13 +2746,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:14">
       <c r="B53" s="3">
-        <f>H53*3</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>137</v>
@@ -2740,13 +2770,13 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="2:16">
+    <row r="54" spans="2:14">
       <c r="B54" s="3">
-        <f>H54*3</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>140</v>
@@ -2764,13 +2794,13 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:14">
       <c r="B55" s="3">
-        <f>H55*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>143</v>
@@ -2788,13 +2818,16 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:14">
       <c r="B56" s="3">
-        <f>H56*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="C56" s="3" t="s">
+        <v>293</v>
+      </c>
       <c r="D56" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>147</v>
@@ -2812,40 +2845,40 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="2:16">
-      <c r="B57" s="3">
-        <f>H57*3</f>
+    <row r="57" spans="2:14" s="6" customFormat="1">
+      <c r="B57" s="6">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="H57" s="3">
-        <v>1</v>
-      </c>
-      <c r="I57" s="3" t="s">
+      <c r="H57" s="6">
+        <v>1</v>
+      </c>
+      <c r="I57" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="2:16">
+    <row r="58" spans="2:14">
       <c r="B58" s="3">
-        <f>H58*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>153</v>
@@ -2866,13 +2899,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="2:16">
+    <row r="59" spans="2:14">
       <c r="B59" s="3">
-        <f>H59*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>157</v>
@@ -2890,13 +2923,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="2:16">
+    <row r="60" spans="2:14">
       <c r="B60" s="3">
-        <f>H60*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>160</v>
@@ -2914,154 +2947,160 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="2:16">
+    <row r="61" spans="2:14">
       <c r="B61" s="3">
-        <f>H61*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="C61" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>275</v>
+      </c>
       <c r="E61" s="3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="H61" s="3">
         <v>1</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="P61" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="62" spans="2:16">
+        <v>170</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N61" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14">
       <c r="B62" s="3">
-        <f>H62*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>168</v>
+      <c r="D62" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>168</v>
+        <v>34</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="H62" s="3">
         <v>1</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="M62" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N62" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14">
       <c r="B63" s="3">
-        <f>H63*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="C63" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H63" s="3">
+        <v>1</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14">
+      <c r="B64" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H63" s="3">
-        <v>1</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="2:16">
-      <c r="B64" s="3">
-        <f>H64*3</f>
+      <c r="E64" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H64" s="3">
+        <v>1</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="B65" s="3">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H64" s="3">
-        <v>1</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="B65" s="3">
-        <f>H65*3</f>
+      <c r="E65" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H65" s="3">
+        <v>1</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="B66" s="3">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H65" s="3">
-        <v>1</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="B66" s="3">
-        <f>H66*3</f>
-        <v>3</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E66" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>186</v>
@@ -3070,95 +3109,95 @@
         <v>1</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="B67" s="3">
-        <f>H67*3</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="H67" s="3">
         <v>1</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="B68" s="3">
-        <f>H68*3</f>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="30">
+      <c r="A69" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="B70" s="3">
+        <v>1</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H70" s="3">
+        <v>1</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" s="8" customFormat="1">
+      <c r="B71" s="8">
+        <f>H71*3</f>
         <v>3</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="H68" s="3">
-        <v>1</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="30">
-      <c r="A70" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="B71" s="3">
-        <v>1</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H71" s="3">
-        <v>1</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>146</v>
+      <c r="D71" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H71" s="8">
+        <v>1</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="P71" s="8" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q68"/>
+  <autoFilter ref="A1:Q67"/>
   <hyperlinks>
-    <hyperlink ref="D71" r:id="rId1"/>
+    <hyperlink ref="D70" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Changed PoE controller to variant A.
</commit_message>
<xml_diff>
--- a/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
+++ b/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$68</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="296">
   <si>
     <t>Qty</t>
   </si>
@@ -902,6 +902,12 @@
   </si>
   <si>
     <t>CKN9104CT-ND</t>
+  </si>
+  <si>
+    <t>MAX5984A</t>
+  </si>
+  <si>
+    <t>MAX5984AETI+-ND</t>
   </si>
 </sst>
 </file>
@@ -1301,9 +1307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="146.85546875" defaultRowHeight="15"/>
   <cols>
@@ -3136,68 +3140,71 @@
         <v>193</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="30">
-      <c r="A69" s="5" t="s">
+    <row r="68" spans="1:16" s="8" customFormat="1">
+      <c r="B68" s="8">
+        <f>H68*3</f>
+        <v>3</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H68" s="8">
+        <v>1</v>
+      </c>
+      <c r="I68" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="P68" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="30">
+      <c r="A70" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
-      <c r="B70" s="3">
-        <v>1</v>
-      </c>
-      <c r="C70" s="3" t="s">
+    <row r="71" spans="1:16">
+      <c r="B71" s="3">
+        <v>1</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="F71" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="G71" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H70" s="3">
-        <v>1</v>
-      </c>
-      <c r="I70" s="3" t="s">
+      <c r="H71" s="3">
+        <v>1</v>
+      </c>
+      <c r="I71" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="8" customFormat="1">
-      <c r="B71" s="8">
-        <f>H71*3</f>
-        <v>3</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H71" s="8">
-        <v>1</v>
-      </c>
-      <c r="I71" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="P71" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:Q67"/>
+  <autoFilter ref="A1:Q68"/>
   <hyperlinks>
-    <hyperlink ref="D70" r:id="rId1"/>
+    <hyperlink ref="D71" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Added terminals for connectors to BOM.
</commit_message>
<xml_diff>
--- a/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
+++ b/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$69</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="298">
   <si>
     <t>Qty</t>
   </si>
@@ -908,6 +908,12 @@
   </si>
   <si>
     <t>MAX5984AETI+-ND</t>
+  </si>
+  <si>
+    <t>S9473CT-ND</t>
+  </si>
+  <si>
+    <t>Connector Terminals</t>
   </si>
 </sst>
 </file>
@@ -1305,9 +1311,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="146.85546875" defaultRowHeight="15"/>
   <cols>
@@ -1504,68 +1512,53 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="3">
-        <f t="shared" ref="B7:B38" si="0">H7*3</f>
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
+        <v>296</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>30</v>
+        <v>297</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="B8" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>208</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>34</v>
@@ -1574,10 +1567,10 @@
         <v>35</v>
       </c>
       <c r="H9" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>228</v>
+        <v>36</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>37</v>
@@ -1585,26 +1578,25 @@
     </row>
     <row r="10" spans="1:16">
       <c r="B10" s="3">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H10" s="3">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>37</v>
@@ -1612,26 +1604,25 @@
     </row>
     <row r="11" spans="1:16">
       <c r="B11" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>229</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>250</v>
+        <v>41</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>37</v>
@@ -1639,26 +1630,26 @@
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" ref="B8:B39" si="0">H12*3</f>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H12" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>45</v>
+        <v>250</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>37</v>
@@ -1666,26 +1657,25 @@
     </row>
     <row r="13" spans="1:16">
       <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>37</v>
@@ -1693,26 +1683,25 @@
     </row>
     <row r="14" spans="1:16">
       <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H14" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>37</v>
@@ -1720,161 +1709,155 @@
     </row>
     <row r="15" spans="1:16">
       <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H15" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>242</v>
+        <v>283</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="H16" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="H17" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>60</v>
+        <v>243</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>257</v>
+        <v>217</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H18" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="H19" s="3">
         <v>1</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>67</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="H20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>32</v>
@@ -1882,302 +1865,291 @@
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>274</v>
+        <v>209</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>67</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>274</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>259</v>
+        <v>288</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H23" s="3">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>79</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="H24" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>79</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="H25" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="3">
-        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="3">
         <v>3</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="H28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>270</v>
+        <v>219</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="H29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="H30" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>99</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="H31" s="3">
         <v>3</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>32</v>
@@ -2185,80 +2157,77 @@
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="3">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H32" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>212</v>
+        <v>258</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H33" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="H34" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>32</v>
@@ -2266,68 +2235,65 @@
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H35" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>245</v>
+        <v>108</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="3">
-        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" s="3">
         <v>3</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="3">
-        <v>1</v>
-      </c>
       <c r="I36" s="3" t="s">
-        <v>113</v>
+        <v>245</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="3">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37" s="3">
-        <v>200</v>
+        <v>213</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>29</v>
@@ -2336,10 +2302,10 @@
         <v>30</v>
       </c>
       <c r="H37" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>32</v>
@@ -2347,26 +2313,25 @@
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E38" s="3">
-        <v>22</v>
+        <v>200</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="H38" s="3">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>32</v>
@@ -2374,134 +2339,129 @@
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="3">
-        <f t="shared" ref="B39:B67" si="1">H39*3</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>116</v>
+        <v>222</v>
+      </c>
+      <c r="E39" s="3">
+        <v>22</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="H39" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>260</v>
+        <v>115</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>234</v>
+        <v>116</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H40" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>263</v>
+        <v>234</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>236</v>
+        <v>120</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="2:10">
       <c r="B42" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>215</v>
+        <v>262</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>121</v>
+        <v>263</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>122</v>
+        <v>236</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="3">
-        <f t="shared" si="1"/>
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E43" s="3">
-        <v>33</v>
+        <v>215</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="H43" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>223</v>
+        <v>122</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>32</v>
@@ -2509,26 +2469,25 @@
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>125</v>
+        <v>224</v>
+      </c>
+      <c r="E44" s="3">
+        <v>33</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="H44" s="3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>32</v>
@@ -2536,53 +2495,51 @@
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H45" s="3">
         <v>1</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="2:10">
       <c r="B46" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H46" s="3">
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>37</v>
@@ -2590,41 +2547,39 @@
     </row>
     <row r="47" spans="2:10">
       <c r="B47" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>237</v>
+        <v>129</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="H47" s="3">
         <v>1</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>238</v>
+        <v>130</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="2:10">
       <c r="B48" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>86</v>
@@ -2636,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>89</v>
@@ -2644,14 +2599,13 @@
     </row>
     <row r="49" spans="2:14">
       <c r="B49" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>131</v>
+        <v>239</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>86</v>
@@ -2663,61 +2617,59 @@
         <v>1</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>132</v>
+        <v>240</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="2:14">
       <c r="B50" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="H50" s="3">
         <v>1</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="2:14">
       <c r="B51" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E51" s="3">
-        <v>680</v>
+        <v>225</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H51" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>32</v>
@@ -2725,14 +2677,13 @@
     </row>
     <row r="52" spans="2:14">
       <c r="B52" s="3">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E52" s="3">
-        <v>750</v>
+        <v>680</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>58</v>
@@ -2741,10 +2692,10 @@
         <v>59</v>
       </c>
       <c r="H52" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>32</v>
@@ -2752,74 +2703,76 @@
     </row>
     <row r="53" spans="2:14">
       <c r="B53" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>137</v>
+        <v>227</v>
+      </c>
+      <c r="E53" s="3">
+        <v>750</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="H53" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="2:14">
       <c r="B54" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" ref="B40:B68" si="1">H54*3</f>
+        <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H54" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="2:14">
       <c r="B55" s="3">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>141</v>
       </c>
       <c r="H55" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="2:14">
@@ -2828,79 +2781,73 @@
         <v>3</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H56" s="3">
         <v>1</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" s="6" customFormat="1">
-      <c r="B57" s="6">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14">
+      <c r="B57" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H57" s="6">
-        <v>1</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14">
-      <c r="B58" s="3">
+      <c r="C57" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H57" s="3">
+        <v>1</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" s="6" customFormat="1">
+      <c r="B58" s="6">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H58" s="3">
-        <v>1</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>78</v>
+      <c r="D58" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H58" s="6">
+        <v>1</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="2:14">
@@ -2909,22 +2856,28 @@
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>276</v>
+        <v>287</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H59" s="3">
         <v>1</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="2:14">
@@ -2933,22 +2886,22 @@
         <v>3</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H60" s="3">
         <v>1</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="2:14">
@@ -2957,34 +2910,22 @@
         <v>3</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H61" s="3">
         <v>1</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="M61" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N61" s="3" t="s">
-        <v>16</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="2:14">
@@ -2992,26 +2933,35 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>172</v>
+      <c r="C62" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>34</v>
+        <v>168</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="H62" s="3">
         <v>1</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>37</v>
+        <v>171</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="2:14">
@@ -3019,26 +2969,26 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>174</v>
+      <c r="D63" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>175</v>
+        <v>34</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>176</v>
+        <v>35</v>
       </c>
       <c r="H63" s="3">
         <v>1</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>178</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="2:14">
@@ -3047,22 +2997,25 @@
         <v>3</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H64" s="3">
         <v>1</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -3071,25 +3024,22 @@
         <v>3</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H65" s="3">
         <v>1</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -3098,13 +3048,13 @@
         <v>3</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>186</v>
@@ -3113,7 +3063,10 @@
         <v>1</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -3122,89 +3075,113 @@
         <v>3</v>
       </c>
       <c r="C67" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H67" s="3">
+        <v>1</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="B68" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H67" s="3">
-        <v>1</v>
-      </c>
-      <c r="I67" s="3" t="s">
+      <c r="H68" s="3">
+        <v>1</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="8" customFormat="1">
-      <c r="B68" s="8">
-        <f>H68*3</f>
+    <row r="69" spans="1:16" s="8" customFormat="1">
+      <c r="B69" s="8">
+        <f>H69*3</f>
         <v>3</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C69" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="D69" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E69" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F69" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="G68" s="8" t="s">
+      <c r="G69" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="H68" s="8">
-        <v>1</v>
-      </c>
-      <c r="I68" s="8" t="s">
+      <c r="H69" s="8">
+        <v>1</v>
+      </c>
+      <c r="I69" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="P68" s="8" t="s">
+      <c r="P69" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="30">
-      <c r="A70" s="5" t="s">
+    <row r="71" spans="1:16" ht="30">
+      <c r="A71" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
-      <c r="B71" s="3">
-        <v>1</v>
-      </c>
-      <c r="C71" s="3" t="s">
+    <row r="72" spans="1:16">
+      <c r="B72" s="3">
+        <v>1</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="F72" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G71" s="3" t="s">
+      <c r="G72" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H71" s="3">
-        <v>1</v>
-      </c>
-      <c r="I71" s="3" t="s">
+      <c r="H72" s="3">
+        <v>1</v>
+      </c>
+      <c r="I72" s="3" t="s">
         <v>146</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q68"/>
+  <autoFilter ref="A1:Q69"/>
   <hyperlinks>
-    <hyperlink ref="D71" r:id="rId1"/>
+    <hyperlink ref="D72" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Text fixed and ready to order.
</commit_message>
<xml_diff>
--- a/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
+++ b/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="299">
   <si>
     <t>Qty</t>
   </si>
@@ -826,9 +826,6 @@
   </si>
   <si>
     <t>PCE3929CT-ND</t>
-  </si>
-  <si>
-    <t>PCE3497CT-ND </t>
   </si>
   <si>
     <t>1N4448W-FDICT-ND</t>
@@ -914,6 +911,12 @@
   </si>
   <si>
     <t>Connector Terminals</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>PCE3497CT-ND</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="146.85546875" defaultRowHeight="15"/>
@@ -1394,7 +1397,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>12</v>
@@ -1448,7 +1451,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>21</v>
@@ -1515,10 +1518,10 @@
         <v>180</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="H7" s="3">
         <v>53</v>
@@ -1630,7 +1633,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="3">
-        <f t="shared" ref="B8:B39" si="0">H12*3</f>
+        <f t="shared" ref="B12" si="0">H12*3</f>
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1738,10 +1741,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>52</v>
@@ -1894,10 +1897,10 @@
         <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>67</v>
@@ -1923,10 +1926,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>74</v>
@@ -2111,7 +2114,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>96</v>
@@ -2628,7 +2631,7 @@
         <v>10</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>131</v>
@@ -2643,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>132</v>
+        <v>297</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>37</v>
@@ -2729,11 +2732,11 @@
     </row>
     <row r="54" spans="2:14">
       <c r="B54" s="3">
-        <f t="shared" ref="B40:B68" si="1">H54*3</f>
+        <f t="shared" ref="B54:B68" si="1">H54*3</f>
         <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>137</v>
@@ -2757,7 +2760,7 @@
         <v>6</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>140</v>
@@ -2781,7 +2784,7 @@
         <v>3</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>143</v>
@@ -2805,10 +2808,10 @@
         <v>3</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>147</v>
@@ -2832,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>149</v>
@@ -2856,10 +2859,10 @@
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>153</v>
@@ -2886,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>157</v>
@@ -2910,7 +2913,7 @@
         <v>3</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>160</v>
@@ -2934,10 +2937,10 @@
         <v>3</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>168</v>
@@ -2970,7 +2973,7 @@
         <v>3</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>172</v>
@@ -2997,7 +3000,7 @@
         <v>3</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>174</v>
@@ -3024,7 +3027,7 @@
         <v>3</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>179</v>
@@ -3048,7 +3051,7 @@
         <v>3</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>185</v>
@@ -3075,7 +3078,7 @@
         <v>3</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>189</v>
@@ -3099,7 +3102,7 @@
         <v>3</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>191</v>
@@ -3123,13 +3126,13 @@
         <v>3</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>164</v>
@@ -3149,7 +3152,7 @@
     </row>
     <row r="71" spans="1:16" ht="30">
       <c r="A71" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:16">
@@ -3157,13 +3160,13 @@
         <v>1</v>
       </c>
       <c r="C72" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="E72" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
Added gerber files for RTx Controller stencil.
</commit_message>
<xml_diff>
--- a/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
+++ b/RTx_Controller_Board/RTxControllerBoardBOM.xlsx
@@ -1316,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A2:A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="146.85546875" defaultRowHeight="15"/>
@@ -1392,385 +1392,466 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1">
-      <c r="B2" s="6">
-        <f>H2*3</f>
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="6" customFormat="1">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="B4" s="3">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="3">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <f>H6*3</f>
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="6">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="B3" s="3">
-        <f>H3*3</f>
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H6" s="3">
         <v>4</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="6" customFormat="1">
-      <c r="B4" s="6">
-        <f>H4*3</f>
+    <row r="7" spans="1:16">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <f>H8*3</f>
         <v>3</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="B5" s="3">
-        <f>H5*3</f>
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="3">
-        <v>6</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="B6" s="3">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="H6" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="B7" s="3">
-        <v>180</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="H7" s="3">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="B8" s="3">
+      <c r="C8" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <f>H9*3</f>
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="B9" s="3">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="B10" s="3">
-        <v>80</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H10" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>228</v>
+        <v>66</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:16">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
       <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
         <v>50</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H12" s="3">
         <v>16</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="B12" s="3">
-        <f t="shared" ref="B12" si="0">H12*3</f>
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="3">
-        <v>4</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
       <c r="B13" s="3">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H13" s="3">
         <v>2</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:16">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
       <c r="B14" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H14" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:16">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
       <c r="B15" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H15" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:16">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
       <c r="B16" s="3">
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
+        <v>47</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
       <c r="B17" s="3">
-        <v>25</v>
+        <f>H17*3</f>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>55</v>
+        <v>229</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>34</v>
@@ -1779,524 +1860,594 @@
         <v>35</v>
       </c>
       <c r="H17" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="1:14">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
       <c r="B18" s="3">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="3">
-        <v>4</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="3">
-        <v>10</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="H19" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="1:14">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
       <c r="B20" s="3">
-        <v>10</v>
+        <f>H20*3</f>
+        <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>218</v>
+        <v>286</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
       <c r="H20" s="3">
         <v>1</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>68</v>
+        <v>156</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
       <c r="B21" s="3">
-        <v>10</v>
+        <f>H21*3</f>
+        <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>209</v>
+        <v>278</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>67</v>
+        <v>179</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>29</v>
+        <v>179</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
       <c r="B22" s="3">
         <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>273</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
       <c r="B23" s="3">
+        <f>H23*3</f>
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
         <v>10</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="3">
-        <v>30</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="H24" s="3">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="1:14">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
       <c r="B25" s="3">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>84</v>
+        <v>228</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
       <c r="B26" s="3">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="H26" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>88</v>
+        <v>243</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
       <c r="B27" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>210</v>
+        <v>256</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H27" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
       <c r="B28" s="3">
         <v>10</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="G28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3">
+        <f>H29*3</f>
+        <v>3</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <f>H30*3</f>
+        <v>12</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H30" s="3">
+        <v>4</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <f>H31*3</f>
+        <v>6</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <f>H32*3</f>
+        <v>3</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" s="3">
+        <v>1</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3">
+        <v>10</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <f>H34*3</f>
+        <v>3</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3">
+        <f>H35*3</f>
+        <v>3</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="H28" s="3">
-        <v>2</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="3">
-        <v>10</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H29" s="3">
-        <v>1</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="3">
-        <v>10</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H30" s="3">
-        <v>2</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10">
-      <c r="B31" s="3">
-        <v>15</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="3">
+      <c r="B36" s="8">
+        <f>H36*3</f>
         <v>3</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="3">
-        <v>15</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="3">
-        <v>3</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="B33" s="3">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H33" s="3">
-        <v>5</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="B34" s="3">
-        <v>10</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="3">
-        <v>1</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="B35" s="3">
-        <v>15</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H35" s="3">
-        <v>4</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="B36" s="3">
-        <v>15</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H36" s="3">
-        <v>3</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10">
+      <c r="C36" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H36" s="8">
+        <v>1</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
       <c r="B37" s="3">
         <v>10</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>112</v>
+        <v>208</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>29</v>
@@ -2308,21 +2459,24 @@
         <v>1</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" spans="1:16">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
       <c r="B38" s="3">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E38" s="3">
-        <v>200</v>
+        <v>211</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>29</v>
@@ -2331,128 +2485,143 @@
         <v>30</v>
       </c>
       <c r="H38" s="3">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="1:16">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
       <c r="B39" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E39" s="3">
-        <v>22</v>
+        <v>220</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H39" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:10">
+    <row r="40" spans="1:16">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
       <c r="B40" s="3">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="H40" s="3">
+        <v>4</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3">
         <v>10</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10">
-      <c r="B41" s="3">
-        <v>5</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>266</v>
+        <v>209</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>234</v>
+        <v>67</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="H41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
       <c r="B42" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>262</v>
+        <v>218</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>263</v>
+        <v>67</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>236</v>
+        <v>68</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
       <c r="B43" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>29</v>
@@ -2464,21 +2633,24 @@
         <v>1</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:10">
+    <row r="44" spans="1:16">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
       <c r="B44" s="3">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E44" s="3">
-        <v>33</v>
+        <v>219</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>58</v>
@@ -2487,516 +2659,559 @@
         <v>59</v>
       </c>
       <c r="H44" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>223</v>
+        <v>95</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:10">
+    <row r="45" spans="1:16">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
       <c r="B45" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="H45" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="J45" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="1:16">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
       <c r="B46" s="3">
         <v>10</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H46" s="3">
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
       <c r="B47" s="3">
         <v>10</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H47" s="3">
         <v>1</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
       <c r="B48" s="3">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>237</v>
+        <v>214</v>
+      </c>
+      <c r="E48" s="3">
+        <v>200</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="H48" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>238</v>
+        <v>114</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
       <c r="B49" s="3">
         <v>10</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>239</v>
+        <v>222</v>
+      </c>
+      <c r="E49" s="3">
+        <v>22</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="H49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>240</v>
+        <v>115</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
       <c r="B50" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>298</v>
+        <v>215</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="H50" s="3">
         <v>1</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>297</v>
+        <v>122</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
       <c r="B51" s="3">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>133</v>
+        <v>224</v>
+      </c>
+      <c r="E51" s="3">
+        <v>33</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H51" s="3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>134</v>
+        <v>223</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:14">
+    <row r="52" spans="1:16">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
       <c r="B52" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E52" s="3">
-        <v>680</v>
+        <v>216</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="H52" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="2:14">
+    <row r="53" spans="1:16">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
       <c r="B53" s="3">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="E53" s="3">
-        <v>750</v>
+        <v>225</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H53" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="2:14">
+    <row r="54" spans="1:16">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
       <c r="B54" s="3">
-        <f t="shared" ref="B54:B68" si="1">H54*3</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>137</v>
+        <v>226</v>
+      </c>
+      <c r="E54" s="3">
+        <v>680</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="H54" s="3">
         <v>4</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14">
+        <v>135</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
       <c r="B55" s="3">
-        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E55" s="3">
+        <v>750</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H55" s="3">
+        <v>7</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3">
+        <v>10</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H56" s="3">
+        <v>1</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3">
+        <v>10</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H57" s="3">
+        <v>1</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" s="6" customFormat="1">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3">
+        <v>10</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H58" s="3">
+        <v>3</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3">
+        <v>5</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H59" s="3">
+        <v>1</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3">
+        <v>10</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H60" s="3">
+        <v>1</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3">
+        <f>H61*3</f>
+        <v>18</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="3">
         <v>6</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H55" s="3">
-        <v>2</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14">
-      <c r="B56" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H56" s="3">
-        <v>1</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14">
-      <c r="B57" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H57" s="3">
-        <v>1</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" s="6" customFormat="1">
-      <c r="B58" s="6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H58" s="6">
-        <v>1</v>
-      </c>
-      <c r="I58" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14">
-      <c r="B59" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H59" s="3">
-        <v>1</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14">
-      <c r="B60" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H60" s="3">
-        <v>1</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14">
-      <c r="B61" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H61" s="3">
-        <v>1</v>
-      </c>
       <c r="I61" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14">
+        <v>27</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" s="6">
+        <v>61</v>
+      </c>
       <c r="B62" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>290</v>
+        <v>204</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>169</v>
+        <v>206</v>
       </c>
       <c r="H62" s="3">
-        <v>1</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="M62" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N62" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
       <c r="B63" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>172</v>
+        <v>180</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>35</v>
+        <v>296</v>
       </c>
       <c r="H63" s="3">
-        <v>1</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" s="6">
+        <v>63</v>
+      </c>
       <c r="B64" s="3">
-        <f t="shared" si="1"/>
+        <f>H64*3</f>
         <v>3</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -3022,133 +3237,177 @@
       </c>
     </row>
     <row r="65" spans="1:16">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
       <c r="B65" s="3">
-        <f t="shared" si="1"/>
+        <f>H65*3</f>
         <v>3</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="H65" s="3">
         <v>1</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:16">
-      <c r="B66" s="3">
-        <f t="shared" si="1"/>
+      <c r="A66" s="6">
+        <v>65</v>
+      </c>
+      <c r="B66" s="6">
+        <f>H66*3</f>
         <v>3</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H66" s="3">
-        <v>1</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>188</v>
-      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="6">
+        <v>1</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
     </row>
     <row r="67" spans="1:16">
-      <c r="B67" s="3">
-        <f t="shared" si="1"/>
+      <c r="A67" s="6">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6">
+        <f>H67*3</f>
         <v>3</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H67" s="3">
-        <v>1</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>190</v>
-      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" s="6">
+        <v>1</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
     </row>
     <row r="68" spans="1:16">
-      <c r="B68" s="3">
-        <f t="shared" si="1"/>
+      <c r="A68" s="6">
+        <v>67</v>
+      </c>
+      <c r="B68" s="6">
+        <f>H68*3</f>
         <v>3</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="H68" s="3">
-        <v>1</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>193</v>
-      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H68" s="6">
+        <v>1</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
     </row>
     <row r="69" spans="1:16" s="8" customFormat="1">
-      <c r="B69" s="8">
+      <c r="A69" s="6">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3">
         <f>H69*3</f>
         <v>3</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G69" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H69" s="8">
-        <v>1</v>
-      </c>
-      <c r="I69" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="P69" s="8" t="s">
-        <v>167</v>
-      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H69" s="3">
+        <v>1</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
     </row>
     <row r="71" spans="1:16" ht="30">
       <c r="A71" s="5" t="s">
@@ -3182,7 +3441,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q69"/>
+  <autoFilter ref="A1:Q69">
+    <sortState ref="A2:P69">
+      <sortCondition ref="C1:C69"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D72" r:id="rId1"/>
   </hyperlinks>

</xml_diff>